<commit_message>
Updated with Integration changes
</commit_message>
<xml_diff>
--- a/samples/virtualan-spring-boot/src/test/resources/virtualan_bdd_testcase_run_manager.xlsx
+++ b/samples/virtualan-spring-boot/src/test/resources/virtualan_bdd_testcase_run_manager.xlsx
@@ -1,12 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24020"/>
   <workbookPr/>
+  <xr:revisionPtr revIDLastSave="57" documentId="11_946C3D24837A7268A57B6A7886915AC5488AB4F0" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3F921E19-20E5-4A3C-AE16-D74F6068FAA9}"/>
+  <bookViews>
+    <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="API-Testing" sheetId="1" r:id="rId4"/>
+    <sheet name="API-Testing" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="191028" calcCompleted="0"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -25,13 +40,13 @@
     <t>ContentType</t>
   </si>
   <si>
-    <t>RequestContents</t>
+    <t>RequestContent</t>
   </si>
   <si>
     <t>ResponseByFields</t>
   </si>
   <si>
-    <t>ResponseContents</t>
+    <t>ResponseContent</t>
   </si>
   <si>
     <t>IncludesByPath</t>
@@ -128,100 +143,658 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="7">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="12.0"/>
+      <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
-      <b/>
-      <sz val="12.0"/>
-      <color rgb="FF008000"/>
-      <name val="Consolas"/>
-    </font>
-    <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
-      <u/>
-      <color rgb="FF0000FF"/>
-    </font>
-    <font>
       <b/>
-      <u/>
-      <sz val="11.0"/>
-      <color rgb="FF1155CC"/>
-      <name val="Inconsolata"/>
-    </font>
-    <font>
-      <sz val="12.0"/>
+      <sz val="12"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
-    <border/>
+  <borders count="10">
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+  <cellXfs count="20">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyFill="1" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="2" fontId="5" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="16">
     <dxf>
-      <font/>
+      <font>
+        <b val="0"/>
+        <color rgb="FF000000"/>
+      </font>
+      <border>
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+        <vertical style="thin">
+          <color rgb="FF000000"/>
+        </vertical>
+        <horizontal style="thin">
+          <color rgb="FF000000"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <color rgb="FF000000"/>
+      </font>
+      <border>
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+        <vertical style="thin">
+          <color rgb="FF000000"/>
+        </vertical>
+        <horizontal style="thin">
+          <color rgb="FF000000"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <color rgb="FF000000"/>
+      </font>
+      <border>
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+        <vertical style="thin">
+          <color rgb="FF000000"/>
+        </vertical>
+        <horizontal style="thin">
+          <color rgb="FF000000"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <color rgb="FF000000"/>
+      </font>
+      <border>
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+        <vertical style="thin">
+          <color rgb="FF000000"/>
+        </vertical>
+        <horizontal style="thin">
+          <color rgb="FF000000"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <color rgb="FF000000"/>
+      </font>
+      <border>
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+        <vertical style="thin">
+          <color rgb="FF000000"/>
+        </vertical>
+        <horizontal style="thin">
+          <color rgb="FF000000"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border>
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+        <vertical style="thin">
+          <color rgb="FF000000"/>
+        </vertical>
+        <horizontal style="thin">
+          <color rgb="FF000000"/>
+        </horizontal>
+      </border>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border>
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+        <vertical style="thin">
+          <color rgb="FF000000"/>
+        </vertical>
+        <horizontal style="thin">
+          <color rgb="FF000000"/>
+        </horizontal>
+      </border>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border>
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+        <vertical style="thin">
+          <color rgb="FF000000"/>
+        </vertical>
+        <horizontal style="thin">
+          <color rgb="FF000000"/>
+        </horizontal>
+      </border>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border>
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+        <vertical style="thin">
+          <color rgb="FF000000"/>
+        </vertical>
+        <horizontal style="thin">
+          <color rgb="FF000000"/>
+        </horizontal>
+      </border>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border>
+        <left/>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+        <vertical style="thin">
+          <color rgb="FF000000"/>
+        </vertical>
+        <horizontal style="thin">
+          <color rgb="FF000000"/>
+        </horizontal>
+      </border>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <border>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <color rgb="FF000000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color rgb="FF000000"/>
+        </vertical>
+        <horizontal style="thin">
+          <color rgb="FF000000"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill patternType="solid">
           <fgColor rgb="FFB7E1CD"/>
           <bgColor rgb="FFB7E1CD"/>
         </patternFill>
       </fill>
-      <border/>
     </dxf>
   </dxfs>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{8A677314-7465-4044-A0BA-49816BDBBBEA}" name="Table2" displayName="Table2" ref="A1:J4" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13" headerRowBorderDxfId="11" tableBorderDxfId="12" totalsRowBorderDxfId="10">
+  <autoFilter ref="A1:J4" xr:uid="{A9500342-2A34-457D-995C-2DA51C621A39}"/>
+  <tableColumns count="10">
+    <tableColumn id="1" xr3:uid="{FA19D31E-03D9-473E-B1EA-7E8F712144F5}" name="TestCaseName" dataDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{5335F966-CF34-4360-BBEB-4CAE8D19B8F7}" name="TestCaseNameDesc" dataDxfId="8"/>
+    <tableColumn id="3" xr3:uid="{6D7AE4E7-F2A0-4CC4-BB6E-EE7F22E0A406}" name="URL" dataDxfId="7"/>
+    <tableColumn id="4" xr3:uid="{CABB6B34-7199-4A85-AEA6-0BB008746702}" name="ContentType" dataDxfId="6"/>
+    <tableColumn id="5" xr3:uid="{FA6FB202-7B69-43FE-9761-E9FE039AFBEC}" name="RequestContent" dataDxfId="5"/>
+    <tableColumn id="6" xr3:uid="{851B6B62-AFDD-4CA7-ACB2-0A67F8A5B244}" name="ResponseByFields" dataDxfId="4"/>
+    <tableColumn id="7" xr3:uid="{3D6B43B3-FDC6-476E-B59B-EEAC338CDC82}" name="ResponseContent" dataDxfId="3"/>
+    <tableColumn id="8" xr3:uid="{8C5E41DF-02B1-4619-9ECA-EDF12C835D9A}" name="IncludesByPath" dataDxfId="2"/>
+    <tableColumn id="9" xr3:uid="{26E4FE9F-772F-41A9-B0CF-D243909DBEBA}" name="Action" dataDxfId="1"/>
+    <tableColumn id="10" xr3:uid="{51320B2B-B3F5-4377-9B03-BEADE430CE70}" name="StatusCode" dataDxfId="0"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -411,133 +984,147 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:J999"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="J3" sqref="J3"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="14.43"/>
-    <col customWidth="1" min="2" max="2" width="28.0"/>
-    <col customWidth="1" min="3" max="3" width="176.14"/>
-    <col customWidth="1" min="4" max="4" width="20.71"/>
-    <col customWidth="1" min="5" max="5" width="27.14"/>
-    <col customWidth="1" min="6" max="6" width="36.0"/>
-    <col customWidth="1" min="7" max="7" width="22.14"/>
+    <col min="1" max="1" width="20.42578125" customWidth="1"/>
+    <col min="2" max="2" width="28" customWidth="1"/>
+    <col min="3" max="3" width="54" customWidth="1"/>
+    <col min="4" max="4" width="20.7109375" customWidth="1"/>
+    <col min="5" max="5" width="51.140625" customWidth="1"/>
+    <col min="6" max="6" width="36" customWidth="1"/>
+    <col min="7" max="7" width="68.85546875" customWidth="1"/>
+    <col min="8" max="8" width="31" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:10">
+      <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="6" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:10" ht="12.75">
+      <c r="A2" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="E2" s="12"/>
+      <c r="F2" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="J2" s="3">
-        <v>200.0</v>
+      <c r="J2" s="11">
+        <v>500</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" s="1" t="s">
+    <row r="3" spans="1:10" ht="234" customHeight="1">
+      <c r="A3" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="E3" s="12"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="13" t="s">
         <v>19</v>
       </c>
+      <c r="H3" s="2"/>
       <c r="I3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="J3" s="1">
-        <v>200.0</v>
+      <c r="J3" s="3">
+        <v>200</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" s="1" t="s">
+    <row r="4" spans="1:10" ht="216.75" customHeight="1">
+      <c r="A4" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="E4" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="F4" s="7"/>
+      <c r="G4" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="H4" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="I4" s="1" t="s">
+      <c r="I4" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="J4" s="1">
-        <v>200.0</v>
+      <c r="J4" s="8">
+        <v>200</v>
       </c>
     </row>
     <row r="20" ht="15.75" customHeight="1"/>
@@ -1522,14 +2109,17 @@
     <row r="999" ht="15.75" customHeight="1"/>
   </sheetData>
   <conditionalFormatting sqref="G2">
-    <cfRule type="notContainsBlanks" dxfId="0" priority="1">
+    <cfRule type="notContainsBlanks" dxfId="15" priority="1">
       <formula>LEN(TRIM(G2))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="C2"/>
-    <hyperlink r:id="rId2" ref="C3"/>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="C3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
   </hyperlinks>
-  <drawing r:id="rId3"/>
+  <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
+  <tableParts count="1">
+    <tablePart r:id="rId3"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>